<commit_message>
Refactor sum/rest logic and generalize step handling
Replaces hardcoded file paths with relative paths, introduces generalized functions get_sum_num and get_rest_num for sum and rest number selection, and refactors the main loop to use dynamic step and condition dictionaries. This improves flexibility and maintainability for handling different calculation steps and conditions.
</commit_message>
<xml_diff>
--- a/sumas o restas pesos.xlsx
+++ b/sumas o restas pesos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4c8a8fd3e0d48bb0/Documentos 1/Documentos/ELAB/Soroban/Codigos/flash_anzan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tlaloc\elopeza\Soroban\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{43F0DAF1-4C2F-4C23-8109-F273B5677FC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B97CE687-3B83-4F4D-8F8C-68064661C042}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED74CF93-F9EB-45EA-8FF6-BDA6176CBF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="8" activeTab="11" xr2:uid="{DAE7EA61-A680-4E4A-9B6B-F7B69FBD9EEC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="8" activeTab="11" xr2:uid="{DAE7EA61-A680-4E4A-9B6B-F7B69FBD9EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Paso 1-3" sheetId="1" r:id="rId1"/>
@@ -140,12 +140,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -467,9 +463,9 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -504,7 +500,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -539,7 +535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -576,7 +572,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -606,7 +602,7 @@
         <v>0.495</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -628,7 +624,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -642,7 +638,7 @@
         <v>0.2475</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -667,7 +663,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -689,7 +685,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -707,7 +703,7 @@
         <v>0.19800000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -721,7 +717,7 @@
         <v>0.14142857142857143</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -744,9 +740,9 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -784,7 +780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -822,7 +818,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -858,7 +854,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -894,7 +890,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -930,7 +926,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -966,7 +962,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1002,7 +998,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1038,7 +1034,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1074,7 +1070,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1110,7 +1106,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1159,9 +1155,9 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1196,7 +1192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1231,7 +1227,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -1269,7 +1265,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1307,7 +1303,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1345,7 +1341,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1383,7 +1379,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1421,7 +1417,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1463,7 +1459,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1506,7 +1502,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1549,7 +1545,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1600,12 +1596,12 @@
   <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1643,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1681,7 +1677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -1690,34 +1686,35 @@
         <v>0.11</v>
       </c>
       <c r="C3">
-        <v>0.01</v>
+        <f>0.36/2</f>
+        <v>0.18</v>
       </c>
       <c r="D3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="E3">
         <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G3">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="J3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K3">
-        <v>7.8333333333333324E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1726,34 +1723,35 @@
         <v>0.11</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D4">
-        <v>0.01</v>
+        <f>0.73/3</f>
+        <v>0.24333333333333332</v>
       </c>
       <c r="E4">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="F4">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I4">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="J4">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K4">
-        <v>7.8333333333333324E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -1762,34 +1760,35 @@
         <v>0.11</v>
       </c>
       <c r="C5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E5">
-        <v>0.01</v>
+        <f>0.78/4</f>
+        <v>0.19500000000000001</v>
       </c>
       <c r="F5">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="G5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I5">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J5">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K5">
-        <v>7.8333333333333324E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1798,34 +1797,35 @@
         <v>0.11</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F6">
-        <v>0.01</v>
+        <f>0.91/5</f>
+        <v>0.182</v>
       </c>
       <c r="G6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="I6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="J6">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="K6">
-        <v>7.8333333333333324E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1834,34 +1834,35 @@
         <v>0.11</v>
       </c>
       <c r="C7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F7">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="G7">
-        <v>0.01</v>
+        <f t="shared" ref="G7:G11" si="1">0.79/5</f>
+        <v>0.158</v>
       </c>
       <c r="H7">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="I7">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="J7">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K7">
-        <v>0.15666666666666665</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1870,34 +1871,39 @@
         <v>0.11</v>
       </c>
       <c r="C8">
-        <v>0.28000000000000003</v>
+        <v>0.18</v>
       </c>
       <c r="D8">
-        <v>0.28499999999999998</v>
+        <f t="shared" ref="D8:D9" si="2">0.73/3</f>
+        <v>0.24333333333333332</v>
       </c>
       <c r="E8">
-        <v>0.19333333333333333</v>
+        <f t="shared" ref="E8:E10" si="3">0.78/4</f>
+        <v>0.19500000000000001</v>
       </c>
       <c r="F8">
-        <v>0.1825</v>
+        <f t="shared" ref="F8:F11" si="4">0.91/5</f>
+        <v>0.182</v>
       </c>
       <c r="G8">
-        <v>0.14499999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.158</v>
       </c>
       <c r="H8">
-        <v>0.01</v>
+        <f t="shared" ref="H8:H11" si="5">0.82/5</f>
+        <v>0.16399999999999998</v>
       </c>
       <c r="I8">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="J8">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K8">
-        <v>0.15666666666666665</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1906,34 +1912,40 @@
         <v>0.11</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D9">
-        <v>0.28499999999999998</v>
+        <f t="shared" si="2"/>
+        <v>0.24333333333333332</v>
       </c>
       <c r="E9">
-        <v>0.19333333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.19500000000000001</v>
       </c>
       <c r="F9">
-        <v>0.1825</v>
+        <f t="shared" si="4"/>
+        <v>0.182</v>
       </c>
       <c r="G9">
-        <v>0.14499999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.158</v>
       </c>
       <c r="H9">
-        <v>0.19333333333333333</v>
+        <f t="shared" si="5"/>
+        <v>0.16399999999999998</v>
       </c>
       <c r="I9">
-        <v>0.01</v>
+        <f t="shared" ref="I9:I11" si="6">0.85/3</f>
+        <v>0.28333333333333333</v>
       </c>
       <c r="J9">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="K9">
-        <v>0.15666666666666665</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1942,34 +1954,40 @@
         <v>0.11</v>
       </c>
       <c r="C10">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D10">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E10">
-        <v>0.19333333333333333</v>
+        <f t="shared" si="3"/>
+        <v>0.19500000000000001</v>
       </c>
       <c r="F10">
-        <v>0.1825</v>
+        <f t="shared" si="4"/>
+        <v>0.182</v>
       </c>
       <c r="G10">
-        <v>0.14499999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.158</v>
       </c>
       <c r="H10">
-        <v>0.19333333333333333</v>
+        <f t="shared" si="5"/>
+        <v>0.16399999999999998</v>
       </c>
       <c r="I10">
-        <v>0.28999999999999998</v>
+        <f t="shared" si="6"/>
+        <v>0.28333333333333333</v>
       </c>
       <c r="J10">
-        <v>0.01</v>
+        <f t="shared" ref="J10:J11" si="7">0.88/2</f>
+        <v>0.44</v>
       </c>
       <c r="K10">
-        <v>0.15666666666666665</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1978,31 +1996,36 @@
         <v>0.11</v>
       </c>
       <c r="C11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="E11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F11">
-        <v>0.1825</v>
+        <f t="shared" si="4"/>
+        <v>0.182</v>
       </c>
       <c r="G11">
-        <v>0.14499999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.158</v>
       </c>
       <c r="H11">
-        <v>0.19333333333333333</v>
+        <f t="shared" si="5"/>
+        <v>0.16399999999999998</v>
       </c>
       <c r="I11">
-        <v>0.28999999999999998</v>
+        <f t="shared" si="6"/>
+        <v>0.28333333333333333</v>
       </c>
       <c r="J11">
-        <v>0.57999999999999996</v>
+        <f t="shared" si="7"/>
+        <v>0.44</v>
       </c>
       <c r="K11">
-        <v>0.05</v>
+        <v>0.91</v>
       </c>
     </row>
   </sheetData>
@@ -2018,9 +2041,9 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2055,7 +2078,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2090,7 +2113,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -2126,7 +2149,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2155,7 +2178,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2176,7 +2199,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2189,7 +2212,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2206,7 +2229,7 @@
         <v>0.2225</v>
       </c>
       <c r="J7">
-        <f t="shared" ref="J7:K10" si="4">0.89/6</f>
+        <f t="shared" ref="J7:J9" si="4">0.89/6</f>
         <v>0.14833333333333334</v>
       </c>
       <c r="K7">
@@ -2214,7 +2237,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2235,7 +2258,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2252,7 +2275,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2265,7 +2288,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2287,9 +2310,9 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2324,7 +2347,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2359,7 +2382,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -2397,7 +2420,7 @@
         <v>0.99</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2433,7 +2456,7 @@
         <v>0.495</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2466,7 +2489,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2495,7 +2518,7 @@
         <v>0.2475</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2517,7 +2540,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2536,7 +2559,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2552,7 +2575,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2565,7 +2588,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2588,9 +2611,9 @@
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2625,7 +2648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2660,7 +2683,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -2694,7 +2717,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -2726,7 +2749,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2756,7 +2779,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2783,7 +2806,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2804,7 +2827,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2822,7 +2845,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2837,7 +2860,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2849,7 +2872,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2871,12 +2894,12 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -2914,7 +2937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2952,7 +2975,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -2990,7 +3013,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3029,7 +3052,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3069,7 +3092,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3110,7 +3133,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3151,7 +3174,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3178,7 +3201,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3210,7 +3233,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3247,7 +3270,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3300,12 +3323,12 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -3343,7 +3366,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3381,7 +3404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -3418,7 +3441,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3456,7 +3479,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3495,7 +3518,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3535,7 +3558,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3575,7 +3598,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3601,7 +3624,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3632,7 +3655,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3668,7 +3691,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3721,12 +3744,12 @@
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -3764,7 +3787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3802,7 +3825,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -3840,7 +3863,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3878,7 +3901,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3916,7 +3939,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3954,7 +3977,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3992,7 +4015,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4034,7 +4057,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4077,7 +4100,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4120,7 +4143,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4174,12 +4197,12 @@
       <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -4217,7 +4240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4255,7 +4278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -4292,7 +4315,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4329,7 +4352,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4366,7 +4389,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4403,7 +4426,7 @@
         <v>7.8333333333333324E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4440,7 +4463,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4480,7 +4503,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4520,7 +4543,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -4559,7 +4582,7 @@
         <v>0.15666666666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -4610,12 +4633,12 @@
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -4653,7 +4676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -4691,7 +4714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <f t="shared" ref="A3:A11" si="0">+A2+1</f>
         <v>1</v>
@@ -4729,7 +4752,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -4767,7 +4790,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -4805,7 +4828,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -4843,7 +4866,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -4881,7 +4904,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -4923,7 +4946,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -4966,7 +4989,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -5009,7 +5032,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>

</xml_diff>